<commit_message>
updated test cases for share skill and manage listings
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>FirstName</t>
   </si>
@@ -112,13 +112,28 @@
     <t>Online</t>
   </si>
   <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>Abcd</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Other</t>
+    <t>Manage</t>
+  </si>
+  <si>
+    <t>ManageListings</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>Video Marketing</t>
   </si>
 </sst>
 </file>
@@ -594,6 +609,50 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3">
+        <v>44585.0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44590.0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -659,10 +718,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -698,6 +757,50 @@
         <v>7.0</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3">
+        <v>44585.0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44590.0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>